<commit_message>
-Phần xem lớp đào tạo tạm ổn -Ghép nối phần xem học viên của Huy -Có xóa 1 số cột k cần trong DB, có lẽ là không ảnh hưởng
</commit_message>
<xml_diff>
--- a/DatabaseExcel/DataBase.xlsx
+++ b/DatabaseExcel/DataBase.xlsx
@@ -9,16 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7776"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7776" activeTab="6"/>
   </bookViews>
   <sheets>
-    <sheet name="HocPhan" sheetId="1" r:id="rId1"/>
-    <sheet name="KQHP" sheetId="6" r:id="rId2"/>
-    <sheet name="HocKi" sheetId="7" r:id="rId3"/>
-    <sheet name="GiangVien" sheetId="2" r:id="rId4"/>
-    <sheet name="Khoa" sheetId="3" r:id="rId5"/>
-    <sheet name="Lop" sheetId="4" r:id="rId6"/>
-    <sheet name="HocVien" sheetId="5" r:id="rId7"/>
+    <sheet name="1Khoa" sheetId="3" r:id="rId1"/>
+    <sheet name="2GiangVien" sheetId="2" r:id="rId2"/>
+    <sheet name="3HocKi" sheetId="7" r:id="rId3"/>
+    <sheet name="4HocPhan" sheetId="1" r:id="rId4"/>
+    <sheet name="5KQHP" sheetId="6" r:id="rId5"/>
+    <sheet name="6Lop" sheetId="4" r:id="rId6"/>
+    <sheet name="7HocVien" sheetId="5" r:id="rId7"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="177">
   <si>
     <t>HP001</t>
   </si>
@@ -368,12 +368,6 @@
   </si>
   <si>
     <t>1271969</t>
-  </si>
-  <si>
-    <t>MaKhoa</t>
-  </si>
-  <si>
-    <t>TenKhoa</t>
   </si>
   <si>
     <t>MT</t>
@@ -967,305 +961,68 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="29.09765625" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.6" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="C1">
-        <v>2</v>
-      </c>
-      <c r="D1">
-        <v>5</v>
-      </c>
-      <c r="E1">
-        <v>45</v>
-      </c>
-      <c r="F1">
-        <v>0.2</v>
-      </c>
-      <c r="G1">
-        <v>0.6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2">
-        <v>5</v>
-      </c>
-      <c r="E2">
-        <v>45</v>
-      </c>
-      <c r="F2">
-        <v>0.2</v>
-      </c>
-      <c r="G2">
-        <v>0.6</v>
-      </c>
-      <c r="H2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
+        <v>111</v>
+      </c>
+      <c r="B2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="D3">
-        <v>5</v>
-      </c>
-      <c r="E3">
-        <v>45</v>
-      </c>
-      <c r="F3">
-        <v>0.2</v>
-      </c>
-      <c r="G3">
-        <v>0.6</v>
-      </c>
-      <c r="H3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="15.6" thickBot="1" x14ac:dyDescent="0.4">
+        <v>113</v>
+      </c>
+      <c r="B3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-      <c r="D4">
-        <v>5</v>
-      </c>
-      <c r="E4">
-        <v>45</v>
-      </c>
-      <c r="F4">
-        <v>0.2</v>
-      </c>
-      <c r="G4">
-        <v>0.6</v>
-      </c>
-      <c r="H4" t="s">
-        <v>23</v>
-      </c>
-      <c r="I4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
+        <v>115</v>
+      </c>
+      <c r="B4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="C5">
-        <v>2</v>
-      </c>
-      <c r="D5">
-        <v>5</v>
-      </c>
-      <c r="E5">
-        <v>45</v>
-      </c>
-      <c r="F5">
-        <v>0.2</v>
-      </c>
-      <c r="G5">
-        <v>0.6</v>
-      </c>
-      <c r="H5" t="s">
-        <v>22</v>
-      </c>
-      <c r="I5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
+        <v>117</v>
+      </c>
+      <c r="B5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="C6">
-        <v>2</v>
-      </c>
-      <c r="D6">
-        <v>5</v>
-      </c>
-      <c r="E6">
-        <v>45</v>
-      </c>
-      <c r="F6">
-        <v>0.2</v>
-      </c>
-      <c r="G6">
-        <v>0.6</v>
-      </c>
-      <c r="H6" t="s">
-        <v>23</v>
-      </c>
-      <c r="I6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
+        <v>119</v>
+      </c>
+      <c r="B6" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="C7">
-        <v>2</v>
-      </c>
-      <c r="D7">
-        <v>5</v>
-      </c>
-      <c r="E7">
-        <v>45</v>
-      </c>
-      <c r="F7">
-        <v>0.2</v>
-      </c>
-      <c r="G7">
-        <v>0.6</v>
-      </c>
-      <c r="H7" t="s">
-        <v>20</v>
-      </c>
-      <c r="I7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="C8">
-        <v>1.5</v>
-      </c>
-      <c r="D8">
-        <v>5</v>
-      </c>
-      <c r="E8">
-        <v>30</v>
-      </c>
-      <c r="F8">
-        <v>0.2</v>
-      </c>
-      <c r="G8">
-        <v>0.6</v>
-      </c>
-      <c r="H8" t="s">
-        <v>21</v>
-      </c>
-      <c r="I8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="C9">
-        <v>1.5</v>
-      </c>
-      <c r="D9">
-        <v>5</v>
-      </c>
-      <c r="E9">
-        <v>30</v>
-      </c>
-      <c r="F9">
-        <v>0.2</v>
-      </c>
-      <c r="G9">
-        <v>0.6</v>
-      </c>
-      <c r="H9" t="s">
-        <v>23</v>
-      </c>
-      <c r="I9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="C10">
-        <v>2</v>
-      </c>
-      <c r="D10">
-        <v>5</v>
-      </c>
-      <c r="E10">
-        <v>45</v>
-      </c>
-      <c r="F10">
-        <v>0.2</v>
-      </c>
-      <c r="G10">
-        <v>0.6</v>
-      </c>
-      <c r="H10" t="s">
-        <v>20</v>
-      </c>
-      <c r="I10" t="s">
-        <v>19</v>
+        <v>87</v>
+      </c>
+      <c r="B7" t="s">
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -1274,278 +1031,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <v>9</v>
-      </c>
-      <c r="B1">
-        <v>9</v>
-      </c>
-      <c r="C1">
-        <v>10</v>
-      </c>
-      <c r="D1" t="s">
-        <v>145</v>
-      </c>
-      <c r="E1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>9</v>
-      </c>
-      <c r="B2">
-        <v>8</v>
-      </c>
-      <c r="C2">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>149</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>9</v>
-      </c>
-      <c r="B3">
-        <v>5</v>
-      </c>
-      <c r="C3">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>153</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>9</v>
-      </c>
-      <c r="B4">
-        <v>6</v>
-      </c>
-      <c r="C4">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s">
-        <v>157</v>
-      </c>
-      <c r="E4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>7</v>
-      </c>
-      <c r="B5">
-        <v>4</v>
-      </c>
-      <c r="C5">
-        <v>10</v>
-      </c>
-      <c r="D5" t="s">
-        <v>161</v>
-      </c>
-      <c r="E5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>8</v>
-      </c>
-      <c r="B6">
-        <v>7.5</v>
-      </c>
-      <c r="C6">
-        <v>7</v>
-      </c>
-      <c r="D6" t="s">
-        <v>145</v>
-      </c>
-      <c r="E6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>10</v>
-      </c>
-      <c r="B7">
-        <v>6.5</v>
-      </c>
-      <c r="C7">
-        <v>8</v>
-      </c>
-      <c r="D7" t="s">
-        <v>149</v>
-      </c>
-      <c r="E7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="B8">
-        <v>8</v>
-      </c>
-      <c r="C8">
-        <v>10</v>
-      </c>
-      <c r="D8" t="s">
-        <v>153</v>
-      </c>
-      <c r="E8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9">
-        <v>9.5</v>
-      </c>
-      <c r="C9">
-        <v>10</v>
-      </c>
-      <c r="D9" t="s">
-        <v>157</v>
-      </c>
-      <c r="E9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10">
-        <v>10</v>
-      </c>
-      <c r="C10">
-        <v>10</v>
-      </c>
-      <c r="D10" t="s">
-        <v>161</v>
-      </c>
-      <c r="E10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="17.796875" customWidth="1"/>
-    <col min="4" max="4" width="20" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" t="s">
-        <v>165</v>
-      </c>
-      <c r="C1" s="5">
-        <v>43352</v>
-      </c>
-      <c r="D1" s="5">
-        <v>43446</v>
-      </c>
-      <c r="E1">
-        <v>2018</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" t="s">
-        <v>166</v>
-      </c>
-      <c r="C2" s="5">
-        <v>43466</v>
-      </c>
-      <c r="D2" s="5">
-        <v>43590</v>
-      </c>
-      <c r="E2">
-        <v>2018</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" t="s">
-        <v>167</v>
-      </c>
-      <c r="C3" s="5">
-        <v>43717</v>
-      </c>
-      <c r="D3" s="5">
-        <v>43811</v>
-      </c>
-      <c r="E3">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" t="s">
-        <v>168</v>
-      </c>
-      <c r="C4" s="5">
-        <v>43831</v>
-      </c>
-      <c r="D4" s="5">
-        <v>43956</v>
-      </c>
-      <c r="E4">
-        <v>2019</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H16"/>
   <sheetViews>
@@ -1997,78 +1482,579 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="17.796875" customWidth="1"/>
+    <col min="4" max="4" width="20" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C1" s="5">
+        <v>43352</v>
+      </c>
+      <c r="D1" s="5">
+        <v>43446</v>
+      </c>
+      <c r="E1">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C2" s="5">
+        <v>43466</v>
+      </c>
+      <c r="D2" s="5">
+        <v>43590</v>
+      </c>
+      <c r="E2">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
+        <v>165</v>
+      </c>
+      <c r="C3" s="5">
+        <v>43717</v>
+      </c>
+      <c r="D3" s="5">
+        <v>43811</v>
+      </c>
+      <c r="E3">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s">
+        <v>166</v>
+      </c>
+      <c r="C4" s="5">
+        <v>43831</v>
+      </c>
+      <c r="D4" s="5">
+        <v>43956</v>
+      </c>
+      <c r="E4">
+        <v>2019</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="29.09765625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="15.6" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>5</v>
+      </c>
+      <c r="E1">
+        <v>45</v>
+      </c>
+      <c r="F1">
+        <v>0.2</v>
+      </c>
+      <c r="G1">
+        <v>0.6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>5</v>
+      </c>
+      <c r="E2">
+        <v>45</v>
+      </c>
+      <c r="F2">
+        <v>0.2</v>
+      </c>
+      <c r="G2">
+        <v>0.6</v>
+      </c>
+      <c r="H2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>5</v>
+      </c>
+      <c r="E3">
+        <v>45</v>
+      </c>
+      <c r="F3">
+        <v>0.2</v>
+      </c>
+      <c r="G3">
+        <v>0.6</v>
+      </c>
+      <c r="H3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15.6" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>5</v>
+      </c>
+      <c r="E4">
+        <v>45</v>
+      </c>
+      <c r="F4">
+        <v>0.2</v>
+      </c>
+      <c r="G4">
+        <v>0.6</v>
+      </c>
+      <c r="H4" t="s">
+        <v>23</v>
+      </c>
+      <c r="I4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>5</v>
+      </c>
+      <c r="E5">
+        <v>45</v>
+      </c>
+      <c r="F5">
+        <v>0.2</v>
+      </c>
+      <c r="G5">
+        <v>0.6</v>
+      </c>
+      <c r="H5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <v>45</v>
+      </c>
+      <c r="F6">
+        <v>0.2</v>
+      </c>
+      <c r="G6">
+        <v>0.6</v>
+      </c>
+      <c r="H6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>5</v>
+      </c>
+      <c r="E7">
+        <v>45</v>
+      </c>
+      <c r="F7">
+        <v>0.2</v>
+      </c>
+      <c r="G7">
+        <v>0.6</v>
+      </c>
+      <c r="H7" t="s">
+        <v>20</v>
+      </c>
+      <c r="I7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C8">
+        <v>1.5</v>
+      </c>
+      <c r="D8">
+        <v>5</v>
+      </c>
+      <c r="E8">
+        <v>30</v>
+      </c>
+      <c r="F8">
+        <v>0.2</v>
+      </c>
+      <c r="G8">
+        <v>0.6</v>
+      </c>
+      <c r="H8" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C9">
+        <v>1.5</v>
+      </c>
+      <c r="D9">
+        <v>5</v>
+      </c>
+      <c r="E9">
+        <v>30</v>
+      </c>
+      <c r="F9">
+        <v>0.2</v>
+      </c>
+      <c r="G9">
+        <v>0.6</v>
+      </c>
+      <c r="H9" t="s">
+        <v>23</v>
+      </c>
+      <c r="I9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <v>5</v>
+      </c>
+      <c r="E10">
+        <v>45</v>
+      </c>
+      <c r="F10">
+        <v>0.2</v>
+      </c>
+      <c r="G10">
+        <v>0.6</v>
+      </c>
+      <c r="H10" t="s">
+        <v>20</v>
+      </c>
+      <c r="I10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>113</v>
-      </c>
-      <c r="B3" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>115</v>
-      </c>
-      <c r="B4" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>117</v>
-      </c>
-      <c r="B5" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>119</v>
-      </c>
-      <c r="B6" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>121</v>
-      </c>
-      <c r="B7" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>87</v>
-      </c>
-      <c r="B8" t="s">
-        <v>124</v>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>9</v>
+      </c>
+      <c r="B1">
+        <v>9</v>
+      </c>
+      <c r="C1">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>9</v>
+      </c>
+      <c r="B2">
+        <v>8</v>
+      </c>
+      <c r="C2">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>147</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>9</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>151</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>155</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>159</v>
+      </c>
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>7.5</v>
+      </c>
+      <c r="C6">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>143</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <v>6.5</v>
+      </c>
+      <c r="C7">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>147</v>
+      </c>
+      <c r="E7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
+        <v>151</v>
+      </c>
+      <c r="E8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>9.5</v>
+      </c>
+      <c r="C9">
+        <v>10</v>
+      </c>
+      <c r="D9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>10</v>
+      </c>
+      <c r="C10">
+        <v>10</v>
+      </c>
+      <c r="D10" t="s">
+        <v>159</v>
+      </c>
+      <c r="E10" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -2088,10 +2074,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C1" t="s">
         <v>29</v>
@@ -2099,10 +2085,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C2" t="s">
         <v>29</v>
@@ -2110,10 +2096,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C3" t="s">
         <v>29</v>
@@ -2121,10 +2107,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C4" t="s">
         <v>29</v>
@@ -2132,10 +2118,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C5" t="s">
         <v>29</v>
@@ -2143,10 +2129,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B6" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C6" t="s">
         <v>29</v>
@@ -2154,10 +2140,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B7" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C7" t="s">
         <v>29</v>
@@ -2165,10 +2151,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B8" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C8" t="s">
         <v>29</v>
@@ -2176,10 +2162,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B9" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C9" t="s">
         <v>29</v>
@@ -2187,10 +2173,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B10" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C10" t="s">
         <v>29</v>
@@ -2205,8 +2191,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2218,16 +2204,16 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C1" t="s">
         <v>145</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>146</v>
-      </c>
-      <c r="C1" t="s">
-        <v>147</v>
-      </c>
-      <c r="D1" t="s">
-        <v>148</v>
       </c>
       <c r="E1">
         <v>903555777</v>
@@ -2239,21 +2225,21 @@
         <v>35950</v>
       </c>
       <c r="H1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C2" t="s">
         <v>149</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>150</v>
-      </c>
-      <c r="C2" t="s">
-        <v>151</v>
-      </c>
-      <c r="D2" t="s">
-        <v>152</v>
       </c>
       <c r="E2">
         <v>903555666</v>
@@ -2265,21 +2251,21 @@
         <v>34977</v>
       </c>
       <c r="H2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C3" t="s">
         <v>153</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
         <v>154</v>
-      </c>
-      <c r="C3" t="s">
-        <v>155</v>
-      </c>
-      <c r="D3" t="s">
-        <v>156</v>
       </c>
       <c r="E3">
         <v>903789777</v>
@@ -2291,21 +2277,21 @@
         <v>34856</v>
       </c>
       <c r="H3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>155</v>
+      </c>
+      <c r="B4" t="s">
+        <v>156</v>
+      </c>
+      <c r="C4" t="s">
         <v>157</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
         <v>158</v>
-      </c>
-      <c r="C4" t="s">
-        <v>159</v>
-      </c>
-      <c r="D4" t="s">
-        <v>160</v>
       </c>
       <c r="E4">
         <v>902565656</v>
@@ -2317,21 +2303,21 @@
         <v>35662</v>
       </c>
       <c r="H4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>159</v>
+      </c>
+      <c r="B5" t="s">
+        <v>160</v>
+      </c>
+      <c r="C5" t="s">
         <v>161</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D5" t="s">
         <v>162</v>
-      </c>
-      <c r="C5" t="s">
-        <v>163</v>
-      </c>
-      <c r="D5" t="s">
-        <v>164</v>
       </c>
       <c r="E5">
         <v>903555542</v>
@@ -2343,7 +2329,7 @@
         <v>36502</v>
       </c>
       <c r="H5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bu Bu Update HK_HP_EXCEL
+Cập nhật validate form thêm học kì, học phần
+điều chỉnh Excel học kì
</commit_message>
<xml_diff>
--- a/DatabaseExcel/DataBase.xlsx
+++ b/DatabaseExcel/DataBase.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GITT\QuanLyDiem\DatabaseExcel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GITHUB\QuanLyDiem\DatabaseExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE165129-7D9A-4A49-A7C6-20E5161ECBC9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7770" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7770" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1Khoa" sheetId="3" r:id="rId1"/>
@@ -25,17 +26,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="201">
   <si>
     <t>HP001</t>
   </si>
@@ -532,12 +528,6 @@
     <t>Học Kì 2</t>
   </si>
   <si>
-    <t>Học Kì 3</t>
-  </si>
-  <si>
-    <t>Học Kì 4</t>
-  </si>
-  <si>
     <t>Toán ứng dụng</t>
   </si>
   <si>
@@ -566,12 +556,90 @@
   </si>
   <si>
     <t>PT % TK hướng đối tượng</t>
+  </si>
+  <si>
+    <t>HK005</t>
+  </si>
+  <si>
+    <t>HK006</t>
+  </si>
+  <si>
+    <t>HK007</t>
+  </si>
+  <si>
+    <t>HK008</t>
+  </si>
+  <si>
+    <t>HK009</t>
+  </si>
+  <si>
+    <t>HK010</t>
+  </si>
+  <si>
+    <t>13/8/2016</t>
+  </si>
+  <si>
+    <t>13/8/2017</t>
+  </si>
+  <si>
+    <t>20/1/2016</t>
+  </si>
+  <si>
+    <t>20/1/2017</t>
+  </si>
+  <si>
+    <t>20/1/2020</t>
+  </si>
+  <si>
+    <t>20/5/2016</t>
+  </si>
+  <si>
+    <t>20/5/2017</t>
+  </si>
+  <si>
+    <t>13/1/2017</t>
+  </si>
+  <si>
+    <t>13/1/2018</t>
+  </si>
+  <si>
+    <t>20/1/2018</t>
+  </si>
+  <si>
+    <t>20/5/2018</t>
+  </si>
+  <si>
+    <t>13/8/2019</t>
+  </si>
+  <si>
+    <t>13/1/2019</t>
+  </si>
+  <si>
+    <t>13/8/2018</t>
+  </si>
+  <si>
+    <t>20/1/2019</t>
+  </si>
+  <si>
+    <t>20/5/2019</t>
+  </si>
+  <si>
+    <t>13/1/2020</t>
+  </si>
+  <si>
+    <t>20/5/2020</t>
+  </si>
+  <si>
+    <t>13/8/2015</t>
+  </si>
+  <si>
+    <t>13/1/2016</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -960,7 +1028,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1031,10 +1099,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
@@ -1461,33 +1529,33 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C1" r:id="rId1"/>
-    <hyperlink ref="C2" r:id="rId2"/>
-    <hyperlink ref="C3" r:id="rId3"/>
-    <hyperlink ref="C4" r:id="rId4"/>
-    <hyperlink ref="C5" r:id="rId5"/>
-    <hyperlink ref="C6" r:id="rId6"/>
-    <hyperlink ref="C7" r:id="rId7"/>
-    <hyperlink ref="C8" r:id="rId8"/>
-    <hyperlink ref="C9" r:id="rId9" display="mailto:huongcnttbk@gmail.com"/>
-    <hyperlink ref="C10" r:id="rId10" display="mailto:dhphuong@dut.udn.vn"/>
-    <hyperlink ref="C11" r:id="rId11" display="mailto:dtthoa@dut.udn.vn"/>
-    <hyperlink ref="C12" r:id="rId12"/>
-    <hyperlink ref="C13" r:id="rId13"/>
-    <hyperlink ref="C14" r:id="rId14"/>
-    <hyperlink ref="C15" r:id="rId15"/>
-    <hyperlink ref="C16" r:id="rId16"/>
+    <hyperlink ref="C1" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="C3" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="C4" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="C5" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="C6" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="C7" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="C8" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
+    <hyperlink ref="C9" r:id="rId9" display="mailto:huongcnttbk@gmail.com" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
+    <hyperlink ref="C10" r:id="rId10" display="mailto:dhphuong@dut.udn.vn" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
+    <hyperlink ref="C11" r:id="rId11" display="mailto:dtthoa@dut.udn.vn" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
+    <hyperlink ref="C12" r:id="rId12" xr:uid="{00000000-0004-0000-0100-00000B000000}"/>
+    <hyperlink ref="C13" r:id="rId13" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
+    <hyperlink ref="C14" r:id="rId14" xr:uid="{00000000-0004-0000-0100-00000D000000}"/>
+    <hyperlink ref="C15" r:id="rId15" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
+    <hyperlink ref="C16" r:id="rId16" xr:uid="{00000000-0004-0000-0100-00000F000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1503,14 +1571,14 @@
       <c r="B1" t="s">
         <v>163</v>
       </c>
-      <c r="C1" s="5">
-        <v>43352</v>
-      </c>
-      <c r="D1" s="5">
-        <v>43446</v>
+      <c r="C1" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>200</v>
       </c>
       <c r="E1">
-        <v>2018</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1520,14 +1588,14 @@
       <c r="B2" t="s">
         <v>164</v>
       </c>
-      <c r="C2" s="5">
-        <v>43466</v>
-      </c>
-      <c r="D2" s="5">
-        <v>43590</v>
+      <c r="C2" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>186</v>
       </c>
       <c r="E2">
-        <v>2018</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1535,16 +1603,16 @@
         <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>165</v>
-      </c>
-      <c r="C3" s="5">
-        <v>43717</v>
-      </c>
-      <c r="D3" s="5">
-        <v>43811</v>
+        <v>163</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>188</v>
       </c>
       <c r="E3">
-        <v>2019</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1552,29 +1620,132 @@
         <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>166</v>
-      </c>
-      <c r="C4" s="5">
-        <v>43831</v>
-      </c>
-      <c r="D4" s="5">
-        <v>43956</v>
+        <v>164</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>187</v>
       </c>
       <c r="E4">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>175</v>
+      </c>
+      <c r="B5" t="s">
+        <v>163</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="E5">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>176</v>
+      </c>
+      <c r="B6" t="s">
+        <v>164</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="E6">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>177</v>
+      </c>
+      <c r="B7" t="s">
+        <v>163</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="E7">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>178</v>
+      </c>
+      <c r="B8" t="s">
+        <v>164</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="E8">
         <v>2019</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>179</v>
+      </c>
+      <c r="B9" t="s">
+        <v>163</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="E9">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>180</v>
+      </c>
+      <c r="B10" t="s">
+        <v>164</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="E10">
+        <v>2020</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1587,7 +1758,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C1">
         <v>2</v>
@@ -1616,7 +1787,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C2">
         <v>2</v>
@@ -1645,7 +1816,7 @@
         <v>9</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -1674,7 +1845,7 @@
         <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -1692,7 +1863,7 @@
         <v>0.6</v>
       </c>
       <c r="H4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="I4" t="s">
         <v>4</v>
@@ -1703,7 +1874,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -1721,7 +1892,7 @@
         <v>0.6</v>
       </c>
       <c r="H5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I5" t="s">
         <v>5</v>
@@ -1732,7 +1903,7 @@
         <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -1761,7 +1932,7 @@
         <v>12</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C7">
         <v>2</v>
@@ -1790,7 +1961,7 @@
         <v>13</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C8">
         <v>1.5</v>
@@ -1819,7 +1990,7 @@
         <v>14</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C9">
         <v>1.5</v>
@@ -1848,7 +2019,7 @@
         <v>15</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C10">
         <v>2</v>
@@ -1878,7 +2049,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2063,7 +2234,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2188,12 +2359,10 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Update chức năng ảnh đại diện
ae thêm vào 2 bảng HV va GV 1 trường Image
</commit_message>
<xml_diff>
--- a/DatabaseExcel/DataBase.xlsx
+++ b/DatabaseExcel/DataBase.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GITHUB\QuanLyDiem\DatabaseExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE165129-7D9A-4A49-A7C6-20E5161ECBC9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{F10417BA-B844-4CC2-8029-D7A7074D1373}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7770" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7770" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1Khoa" sheetId="3" r:id="rId1"/>
@@ -1100,18 +1100,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="7" width="20.5703125" customWidth="1"/>
+    <col min="7" max="8" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1133,11 +1133,12 @@
       <c r="G1" s="5">
         <v>28867</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="5"/>
+      <c r="I1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1159,11 +1160,12 @@
       <c r="G2" s="5">
         <v>29233</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="5"/>
+      <c r="I2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1185,11 +1187,12 @@
       <c r="G3" s="5">
         <v>29934</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="5"/>
+      <c r="I3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1211,11 +1214,12 @@
       <c r="G4" s="5">
         <v>29159</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="5"/>
+      <c r="I4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1237,11 +1241,12 @@
       <c r="G5" s="5">
         <v>27683</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="5"/>
+      <c r="I5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1263,11 +1268,12 @@
       <c r="G6" s="5">
         <v>29002</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="5"/>
+      <c r="I6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -1289,11 +1295,12 @@
       <c r="G7" s="5">
         <v>31136</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="5"/>
+      <c r="I7" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -1315,11 +1322,12 @@
       <c r="G8" s="5">
         <v>28874</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" s="5"/>
+      <c r="I8" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -1341,11 +1349,12 @@
       <c r="G9" s="5">
         <v>28885</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" s="5"/>
+      <c r="I9" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -1367,11 +1376,12 @@
       <c r="G10" s="5">
         <v>31413</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H10" s="5"/>
+      <c r="I10" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>75</v>
       </c>
@@ -1393,11 +1403,12 @@
       <c r="G11" s="5">
         <v>25225</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11" s="5"/>
+      <c r="I11" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>81</v>
       </c>
@@ -1419,11 +1430,12 @@
       <c r="G12" s="5">
         <v>25226</v>
       </c>
-      <c r="H12" s="4" t="s">
+      <c r="H12" s="5"/>
+      <c r="I12" s="4" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>88</v>
       </c>
@@ -1445,11 +1457,12 @@
       <c r="G13" s="5">
         <v>25227</v>
       </c>
-      <c r="H13" s="4" t="s">
+      <c r="H13" s="5"/>
+      <c r="I13" s="4" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>93</v>
       </c>
@@ -1471,11 +1484,12 @@
       <c r="G14" s="5">
         <v>25228</v>
       </c>
-      <c r="H14" s="4" t="s">
+      <c r="H14" s="5"/>
+      <c r="I14" s="4" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>99</v>
       </c>
@@ -1497,11 +1511,12 @@
       <c r="G15" s="5">
         <v>25229</v>
       </c>
-      <c r="H15" s="4" t="s">
+      <c r="H15" s="5"/>
+      <c r="I15" s="4" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>105</v>
       </c>
@@ -1523,7 +1538,8 @@
       <c r="G16" s="5">
         <v>25230</v>
       </c>
-      <c r="H16" s="4" t="s">
+      <c r="H16" s="5"/>
+      <c r="I16" s="4" t="s">
         <v>87</v>
       </c>
     </row>
@@ -1554,7 +1570,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
@@ -2360,18 +2376,20 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="24.140625" customWidth="1"/>
     <col min="6" max="6" width="27.42578125" customWidth="1"/>
-    <col min="7" max="7" width="18.85546875" customWidth="1"/>
+    <col min="7" max="8" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>143</v>
       </c>
@@ -2393,11 +2411,12 @@
       <c r="G1" s="5">
         <v>35950</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="5"/>
+      <c r="I1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>147</v>
       </c>
@@ -2419,11 +2438,12 @@
       <c r="G2" s="5">
         <v>34977</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="5"/>
+      <c r="I2" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>151</v>
       </c>
@@ -2445,11 +2465,12 @@
       <c r="G3" s="5">
         <v>34856</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="5"/>
+      <c r="I3" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>155</v>
       </c>
@@ -2471,11 +2492,12 @@
       <c r="G4" s="5">
         <v>35662</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="5"/>
+      <c r="I4" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>159</v>
       </c>
@@ -2497,7 +2519,8 @@
       <c r="G5" s="5">
         <v>36502</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="5"/>
+      <c r="I5" t="s">
         <v>125</v>
       </c>
     </row>

</xml_diff>